<commit_message>
started opensource rocket Sim
</commit_message>
<xml_diff>
--- a/rocketProperties.xlsx
+++ b/rocketProperties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bktf3\Desktop\rocket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAA23CC-3C8C-48C2-8B25-A97DD5916389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F42A3C4-790C-4D8A-A3FD-DB9C91BE2885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{17CB842C-942D-4B28-920E-3B6EF1C909D4}"/>
   </bookViews>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44C454B9-543C-46D5-9EC8-90FFAB00B659}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1176,8 +1176,8 @@
         <v>35</v>
       </c>
       <c r="I23" s="2">
-        <f>0.466*0.16</f>
-        <v>7.4560000000000001E-2</v>
+        <f>0.5*0.16</f>
+        <v>0.08</v>
       </c>
       <c r="L23">
         <f>0.466*0.165</f>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="I32" s="2">
         <f>(I2*I23+I15*I26+I20*I30)/(I2+I15+I20)</f>
-        <v>0.63151938954032261</v>
+        <v>0.63217610902895671</v>
       </c>
       <c r="J32" t="s">
         <v>37</v>
@@ -1443,7 +1443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3389EB6-37DD-4363-B607-B75A9FEA58E6}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added a note to the mass measurements note because the sum of component mass is different from the mass i used for the sim. I probably took out a few stuffings before i launched it?
</commit_message>
<xml_diff>
--- a/rocketProperties.xlsx
+++ b/rocketProperties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bktf3\Desktop\rocket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F42A3C4-790C-4D8A-A3FD-DB9C91BE2885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC7E629-7302-47AA-AF68-D1F656E3BD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{17CB842C-942D-4B28-920E-3B6EF1C909D4}"/>
+    <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="11295" xr2:uid="{17CB842C-942D-4B28-920E-3B6EF1C909D4}"/>
   </bookViews>
   <sheets>
     <sheet name="black" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Bonsuck Koo</author>
+  </authors>
+  <commentList>
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{7ABB4D2F-941D-44E5-90E3-52DE91AC22EC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Bonsuck Koo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+&lt; this is probably the mass I measured after I closed the nose  cap. It weighed less than the sum of the componenets above probably because I put in less stuffing?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="82">
   <si>
@@ -290,7 +324,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,6 +371,19 @@
       <color rgb="FF00B050"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -708,11 +755,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44C454B9-543C-46D5-9EC8-90FFAB00B659}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44C454B9-543C-46D5-9EC8-90FFAB00B659}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1398,7 +1445,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="42.75">
+    <row r="35" spans="1:15" ht="28.5">
       <c r="G35" s="4" t="s">
         <v>76</v>
       </c>
@@ -1436,6 +1483,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>